<commit_message>
Correction nom site + courbe d'abondance et Pareto
</commit_message>
<xml_diff>
--- a/RAW1/Soil_R.xlsx
+++ b/RAW1/Soil_R.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumniumonsac-my.sharepoint.com/personal/151201_umons_ac_be/Documents/UMONS/MA2/MEMOIRE/Statistique/R/MEMOIRE/RAW1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumniumonsac-my.sharepoint.com/personal/151201_umons_ac_be/Documents/UMONS/MA2/MEMOIRE/Statistique/R/STAT-MEMOIRE/RAW1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="8_{16C2DE22-5167-4D4C-A02D-D4A7C4A56550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E6676A9-134F-432F-B9FB-3995458FE66C}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="8_{16C2DE22-5167-4D4C-A02D-D4A7C4A56550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA790E13-D48E-4BE1-A818-E3C0666FADCD}"/>
   <bookViews>
-    <workbookView xWindow="35295" yWindow="1575" windowWidth="21600" windowHeight="11385" xr2:uid="{ED16C615-2DF0-442E-9261-D5D8A80DE51C}"/>
+    <workbookView xWindow="468" yWindow="5268" windowWidth="17280" windowHeight="8964" xr2:uid="{ED16C615-2DF0-442E-9261-D5D8A80DE51C}"/>
   </bookViews>
   <sheets>
     <sheet name="R" sheetId="1" r:id="rId1"/>
@@ -40,9 +40,6 @@
     <t>Chasse Cambier</t>
   </si>
   <si>
-    <t>Mel Légumes</t>
-  </si>
-  <si>
     <t>Jean d'Avesnes</t>
   </si>
   <si>
@@ -52,15 +49,9 @@
     <t>Jardin Suspendu</t>
   </si>
   <si>
-    <t>Siège social</t>
-  </si>
-  <si>
     <t>Abbaye St-Denis</t>
   </si>
   <si>
-    <t>École de l’Espérance</t>
-  </si>
-  <si>
     <t>Fond du petit marais</t>
   </si>
   <si>
@@ -73,9 +64,6 @@
     <t>Parc du Beffroi</t>
   </si>
   <si>
-    <t>Rue de l'Égalité</t>
-  </si>
-  <si>
     <t>Stievenart</t>
   </si>
   <si>
@@ -116,6 +104,18 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Mel Legumes</t>
+  </si>
+  <si>
+    <t>Rue de l'Egalite</t>
+  </si>
+  <si>
+    <t>Siege social</t>
+  </si>
+  <si>
+    <t>Ecole de l'Esperance</t>
   </si>
 </sst>
 </file>
@@ -349,7 +349,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -649,62 +649,62 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J20" sqref="J20"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="25.375" customWidth="1"/>
-    <col min="2" max="12" width="14.375" customWidth="1"/>
-    <col min="13" max="13" width="25.375" customWidth="1"/>
-    <col min="14" max="14" width="24.625" customWidth="1"/>
-    <col min="15" max="15" width="26.875" customWidth="1"/>
-    <col min="16" max="16" width="21.625" customWidth="1"/>
+    <col min="1" max="1" width="28.3984375" customWidth="1"/>
+    <col min="2" max="12" width="14.3984375" customWidth="1"/>
+    <col min="13" max="13" width="25.3984375" customWidth="1"/>
+    <col min="14" max="14" width="24.59765625" customWidth="1"/>
+    <col min="15" max="15" width="26.8984375" customWidth="1"/>
+    <col min="16" max="16" width="21.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="4" customFormat="1">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="J1" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="K1" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="L1" s="32" t="s">
         <v>22</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" s="32" t="s">
-        <v>26</v>
       </c>
       <c r="N1" s="5"/>
       <c r="P1" s="5"/>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="33" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" s="6">
         <v>6.27</v>
@@ -745,7 +745,7 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="33" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B3" s="6">
         <v>6.33</v>
@@ -827,7 +827,7 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="33" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="B5" s="6">
         <v>7.91</v>
@@ -868,7 +868,7 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="33" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B6" s="6">
         <v>3.18</v>
@@ -909,7 +909,7 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="33" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="6">
         <v>8.14</v>
@@ -950,7 +950,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="33" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="6">
         <v>6.06</v>
@@ -991,7 +991,7 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="33" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" s="6">
         <v>7.87</v>
@@ -1032,7 +1032,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="33" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B10" s="6">
         <v>6.44</v>
@@ -1073,7 +1073,7 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="33" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B11" s="7">
         <v>11.2</v>
@@ -1114,7 +1114,7 @@
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="33" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B12" s="7">
         <v>11.4</v>
@@ -1155,7 +1155,7 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="33" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B13" s="6">
         <v>8.3800000000000008</v>
@@ -1196,7 +1196,7 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="33" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B14" s="6">
         <v>5.8</v>
@@ -1237,7 +1237,7 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="33" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B15" s="6">
         <v>7.46</v>
@@ -1276,9 +1276,9 @@
       <c r="M15" s="7"/>
       <c r="O15" s="7"/>
     </row>
-    <row r="16" spans="1:16" ht="16.5" thickBot="1">
+    <row r="16" spans="1:16" ht="16.2" thickBot="1">
       <c r="A16" s="33" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B16" s="18">
         <v>4.53</v>

</xml_diff>

<commit_message>
Exportation tableau abondance par site
</commit_message>
<xml_diff>
--- a/RAW1/Soil_R.xlsx
+++ b/RAW1/Soil_R.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="52" documentId="8_{16C2DE22-5167-4D4C-A02D-D4A7C4A56550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA790E13-D48E-4BE1-A818-E3C0666FADCD}"/>
   <bookViews>
-    <workbookView xWindow="468" yWindow="5268" windowWidth="17280" windowHeight="8964" xr2:uid="{ED16C615-2DF0-442E-9261-D5D8A80DE51C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ED16C615-2DF0-442E-9261-D5D8A80DE51C}"/>
   </bookViews>
   <sheets>
     <sheet name="R" sheetId="1" r:id="rId1"/>
@@ -649,17 +649,17 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="28.3984375" customWidth="1"/>
-    <col min="2" max="12" width="14.3984375" customWidth="1"/>
-    <col min="13" max="13" width="25.3984375" customWidth="1"/>
-    <col min="14" max="14" width="24.59765625" customWidth="1"/>
-    <col min="15" max="15" width="26.8984375" customWidth="1"/>
-    <col min="16" max="16" width="21.59765625" customWidth="1"/>
+    <col min="1" max="1" width="28.375" customWidth="1"/>
+    <col min="2" max="12" width="14.375" customWidth="1"/>
+    <col min="13" max="13" width="25.375" customWidth="1"/>
+    <col min="14" max="14" width="24.625" customWidth="1"/>
+    <col min="15" max="15" width="26.875" customWidth="1"/>
+    <col min="16" max="16" width="21.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="4" customFormat="1">
@@ -1276,7 +1276,7 @@
       <c r="M15" s="7"/>
       <c r="O15" s="7"/>
     </row>
-    <row r="16" spans="1:16" ht="16.2" thickBot="1">
+    <row r="16" spans="1:16" ht="16.5" thickBot="1">
       <c r="A16" s="33" t="s">
         <v>7</v>
       </c>

</xml_diff>